<commit_message>
added code for population and dataset
</commit_message>
<xml_diff>
--- a/EICV dash/children_population.xlsx
+++ b/EICV dash/children_population.xlsx
@@ -41,112 +41,112 @@
     <t>City of Kigali</t>
   </si>
   <si>
-    <t xml:space="preserve">  Nyarugenge</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Gasabo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Kicukiro</t>
-  </si>
-  <si>
     <t>Southern Province</t>
   </si>
   <si>
-    <t xml:space="preserve">  Nyanza</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Gisagara</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Nyaruguru</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Huye</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Nyamagabe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Ruhango</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Muhanga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Kamonyi</t>
-  </si>
-  <si>
     <t>Western Province</t>
   </si>
   <si>
-    <t xml:space="preserve">  Karongi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Rutsiro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Rubavu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Nyabihu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Ngororero</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Rusizi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Nyamasheke</t>
-  </si>
-  <si>
     <t>Northern Province</t>
   </si>
   <si>
-    <t xml:space="preserve">  Rulindo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Gakenke</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Musanze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Burera</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Gicumbi</t>
-  </si>
-  <si>
     <t>Eastern Province</t>
   </si>
   <si>
-    <t xml:space="preserve">  Rwamagana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Nyagatare</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Gatsibo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Kayonza</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Kirehe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Ngoma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Bugesera</t>
-  </si>
-  <si>
     <t>district</t>
   </si>
   <si>
     <t>province</t>
+  </si>
+  <si>
+    <t>Nyarugenge</t>
+  </si>
+  <si>
+    <t>Gasabo</t>
+  </si>
+  <si>
+    <t>Kicukiro</t>
+  </si>
+  <si>
+    <t>Nyanza</t>
+  </si>
+  <si>
+    <t>Gisagara</t>
+  </si>
+  <si>
+    <t>Nyaruguru</t>
+  </si>
+  <si>
+    <t>Huye</t>
+  </si>
+  <si>
+    <t>Nyamagabe</t>
+  </si>
+  <si>
+    <t>Ruhango</t>
+  </si>
+  <si>
+    <t>Muhanga</t>
+  </si>
+  <si>
+    <t>Kamonyi</t>
+  </si>
+  <si>
+    <t>Karongi</t>
+  </si>
+  <si>
+    <t>Rutsiro</t>
+  </si>
+  <si>
+    <t>Rubavu</t>
+  </si>
+  <si>
+    <t>Nyabihu</t>
+  </si>
+  <si>
+    <t>Ngororero</t>
+  </si>
+  <si>
+    <t>Rusizi</t>
+  </si>
+  <si>
+    <t>Nyamasheke</t>
+  </si>
+  <si>
+    <t>Rulindo</t>
+  </si>
+  <si>
+    <t>Gakenke</t>
+  </si>
+  <si>
+    <t>Musanze</t>
+  </si>
+  <si>
+    <t>Burera</t>
+  </si>
+  <si>
+    <t>Gicumbi</t>
+  </si>
+  <si>
+    <t>Rwamagana</t>
+  </si>
+  <si>
+    <t>Nyagatare</t>
+  </si>
+  <si>
+    <t>Gatsibo</t>
+  </si>
+  <si>
+    <t>Kayonza</t>
+  </si>
+  <si>
+    <t>Kirehe</t>
+  </si>
+  <si>
+    <t>Ngoma</t>
+  </si>
+  <si>
+    <t>Bugesera</t>
   </si>
 </sst>
 </file>
@@ -221,11 +221,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -509,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:XFD38"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -519,16 +519,16 @@
     <col min="2" max="2" width="15.77734375" style="3" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="31.5546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="3" customWidth="1"/>
     <col min="6" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>39</v>
+        <v>10</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -547,13 +547,13 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>5896555</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>2949946</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>2946609</v>
       </c>
     </row>
@@ -564,13 +564,13 @@
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>661634</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>326706</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>334928</v>
       </c>
     </row>
@@ -579,15 +579,15 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="5">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4">
         <v>138222</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>68327</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>69895</v>
       </c>
     </row>
@@ -596,15 +596,15 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="5">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4">
         <v>347276</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>171636</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>175640</v>
       </c>
     </row>
@@ -613,542 +613,542 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="5">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4">
         <v>176136</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>86743</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>89393</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="5">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4">
         <v>1333741</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>671495</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>662246</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="5">
+        <v>14</v>
+      </c>
+      <c r="C8" s="4">
         <v>165293</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>83664</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>81629</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="5">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4">
         <v>187559</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>94849</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>92710</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="5">
+        <v>16</v>
+      </c>
+      <c r="C10" s="4">
         <v>150844</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>75558</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>75286</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="5">
+        <v>17</v>
+      </c>
+      <c r="C11" s="4">
         <v>163147</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>81978</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>81169</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C12" s="5">
+        <v>18</v>
+      </c>
+      <c r="C12" s="4">
         <v>162305</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>81351</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>80954</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="5">
+        <v>19</v>
+      </c>
+      <c r="C13" s="4">
         <v>159595</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>81102</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>78493</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C14" s="5">
+        <v>20</v>
+      </c>
+      <c r="C14" s="4">
         <v>148152</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>74180</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>73972</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="5">
+        <v>21</v>
+      </c>
+      <c r="C15" s="4">
         <v>196846</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>98813</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>98033</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="5">
+        <v>6</v>
+      </c>
+      <c r="C16" s="4">
         <v>1355666</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>678050</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <v>677616</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="5">
+        <v>22</v>
+      </c>
+      <c r="C17" s="4">
         <v>169835</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>85673</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <v>84162</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="5">
+        <v>23</v>
+      </c>
+      <c r="C18" s="4">
         <v>170344</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <v>85296</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="4">
         <v>85048</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="5">
+        <v>24</v>
+      </c>
+      <c r="C19" s="4">
         <v>259552</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <v>128904</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <v>130648</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="5">
+        <v>25</v>
+      </c>
+      <c r="C20" s="4">
         <v>148252</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="4">
         <v>73992</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <v>74260</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C21" s="5">
+        <v>26</v>
+      </c>
+      <c r="C21" s="4">
         <v>172563</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="4">
         <v>85712</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="4">
         <v>86851</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="5">
+        <v>27</v>
+      </c>
+      <c r="C22" s="4">
         <v>229264</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="4">
         <v>115440</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="4">
         <v>113824</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="3" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="5">
+        <v>28</v>
+      </c>
+      <c r="C23" s="4">
         <v>205856</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="4">
         <v>103033</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="4">
         <v>102823</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="3" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="5">
+        <v>7</v>
+      </c>
+      <c r="C24" s="4">
         <v>888802</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="4">
         <v>442442</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="4">
         <v>446360</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="5">
+        <v>29</v>
+      </c>
+      <c r="C25" s="4">
         <v>156253</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="4">
         <v>78031</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="4">
         <v>78222</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="3" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="5">
+        <v>30</v>
+      </c>
+      <c r="C26" s="4">
         <v>155697</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="4">
         <v>77817</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="4">
         <v>77880</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="3" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="5">
+        <v>31</v>
+      </c>
+      <c r="C27" s="4">
         <v>206471</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="4">
         <v>102243</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27" s="4">
         <v>104228</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="3" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C28" s="5">
+        <v>32</v>
+      </c>
+      <c r="C28" s="4">
         <v>175346</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="4">
         <v>87118</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="4">
         <v>88228</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="3" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C29" s="5">
+        <v>33</v>
+      </c>
+      <c r="C29" s="4">
         <v>195035</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="4">
         <v>97233</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="4">
         <v>97802</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="3" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C30" s="5">
+        <v>8</v>
+      </c>
+      <c r="C30" s="4">
         <v>1656712</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="4">
         <v>831253</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30" s="4">
         <v>825459</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="3" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="5">
+        <v>34</v>
+      </c>
+      <c r="C31" s="4">
         <v>210912</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="4">
         <v>105321</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E31" s="4">
         <v>105591</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="3" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="5">
+        <v>35</v>
+      </c>
+      <c r="C32" s="4">
         <v>311745</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="4">
         <v>156863</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="4">
         <v>154882</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="3" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="5">
+        <v>36</v>
+      </c>
+      <c r="C33" s="4">
         <v>258449</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="4">
         <v>129078</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E33" s="4">
         <v>129371</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="3" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="5">
+        <v>37</v>
+      </c>
+      <c r="C34" s="4">
         <v>214598</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D34" s="4">
         <v>108079</v>
       </c>
-      <c r="E34" s="5">
+      <c r="E34" s="4">
         <v>106519</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="3" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="5">
+        <v>38</v>
+      </c>
+      <c r="C35" s="4">
         <v>215324</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D35" s="4">
         <v>107989</v>
       </c>
-      <c r="E35" s="5">
+      <c r="E35" s="4">
         <v>107335</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="3" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" s="5">
+        <v>39</v>
+      </c>
+      <c r="C36" s="4">
         <v>188047</v>
       </c>
-      <c r="D36" s="5">
+      <c r="D36" s="4">
         <v>94807</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E36" s="4">
         <v>93240</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="3" t="s">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" s="5">
+        <v>40</v>
+      </c>
+      <c r="C37" s="4">
         <v>257637</v>
       </c>
-      <c r="D37" s="5">
+      <c r="D37" s="4">
         <v>129116</v>
       </c>
-      <c r="E37" s="5">
+      <c r="E37" s="4">
         <v>128521</v>
       </c>
     </row>

</xml_diff>